<commit_message>
Solve Problmes From Level 2 Arrays
</commit_message>
<xml_diff>
--- a/Practice Only/DSA PPCDING.xlsx
+++ b/Practice Only/DSA PPCDING.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\DSA\Practice Only\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ED8803-4E45-4B2D-AF5F-0A97326BBB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A476A822-0295-497E-8613-0F3A4D8C810B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="1450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2884" uniqueCount="1455">
   <si>
     <t>https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/middle-of-a-linked-list/ojquestion</t>
   </si>
@@ -4381,6 +4381,21 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Lots Of Edge Cases Be Careful While Solving</t>
+  </si>
+  <si>
+    <t>Add To First And Last Index And Do Prefix Sum</t>
+  </si>
+  <si>
+    <t>Two Pointer At First And Last Index Think Of How To Move The Pointers</t>
+  </si>
+  <si>
+    <t>Do In O(n)</t>
+  </si>
+  <si>
+    <t>Next Permutation num-&gt; string then to back again numString to long by -&gt;stol</t>
   </si>
 </sst>
 </file>
@@ -4824,15 +4839,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:N740"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="C448" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C465" sqref="C465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.125" customWidth="1"/>
-    <col min="3" max="3" width="104.625" customWidth="1"/>
+    <col min="3" max="3" width="62.375" customWidth="1"/>
     <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="71.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
@@ -14391,6 +14407,9 @@
       <c r="D463" s="7" t="s">
         <v>1449</v>
       </c>
+      <c r="E463" t="s">
+        <v>1450</v>
+      </c>
       <c r="M463" t="s">
         <v>898</v>
       </c>
@@ -14412,6 +14431,9 @@
       <c r="D464" s="7" t="s">
         <v>1449</v>
       </c>
+      <c r="E464" t="s">
+        <v>1451</v>
+      </c>
       <c r="M464" t="s">
         <v>900</v>
       </c>
@@ -14454,6 +14476,9 @@
       <c r="D466" s="7" t="s">
         <v>1449</v>
       </c>
+      <c r="E466" t="s">
+        <v>1452</v>
+      </c>
       <c r="M466" t="s">
         <v>904</v>
       </c>
@@ -14475,6 +14500,9 @@
       <c r="D467" s="7" t="s">
         <v>1449</v>
       </c>
+      <c r="E467" t="s">
+        <v>1453</v>
+      </c>
       <c r="M467" t="s">
         <v>906</v>
       </c>
@@ -14495,6 +14523,9 @@
       </c>
       <c r="D468" s="7" t="s">
         <v>1449</v>
+      </c>
+      <c r="E468" t="s">
+        <v>1454</v>
       </c>
       <c r="M468" t="s">
         <v>908</v>

</xml_diff>